<commit_message>
Finalização da criação e inserção de registros nas tabelas.
Finalização da criação e inserção de registros nas tabelas de produtos e cadastro de clientes e juntamente da criação da pasta de projetos com interação de comando do Oracle Datanase pelo SQL Developer.
</commit_message>
<xml_diff>
--- a/Oracle/Inserção de registros na tabela/Arquivo auxiliar de produtos.xlsx
+++ b/Oracle/Inserção de registros na tabela/Arquivo auxiliar de produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsempreboni\Downloads\arquivos-aula-3\Arquivos - Aula 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E86986-4A74-4250-A748-DB9D650F664E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809A606C-EB83-42EA-B08C-270477286674}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="74">
   <si>
     <t>Sabor da Montanha - 700 ml - Uva</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Morango</t>
+  </si>
+  <si>
+    <t>Instrução SQL utilitária</t>
   </si>
 </sst>
 </file>
@@ -685,7 +688,9 @@
       <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">

</xml_diff>